<commit_message>
Fix DXF, add BOM PDF and board labels image.
DXF used to show traces, not anymore.
An image file has been added for reference when populating the board.
BOM PDF only contains the parts required to populate the board and make
a basic robot. Good to be used as a check list.
</commit_message>
<xml_diff>
--- a/Robot Board v003 BOM v2.xlsx
+++ b/Robot Board v003 BOM v2.xlsx
@@ -828,16 +828,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="46" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="46" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7" style="36" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" customWidth="1"/>
-    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -893,7 +893,7 @@
         <v>3.75</v>
       </c>
       <c r="F2" s="6">
-        <f>C2*E2</f>
+        <f t="shared" ref="F2:F25" si="0">C2*E2</f>
         <v>37.5</v>
       </c>
       <c r="G2" s="6" t="s">
@@ -906,7 +906,7 @@
         <v>11</v>
       </c>
       <c r="J2" s="5">
-        <f>A2</f>
+        <f t="shared" ref="J2:J25" si="1">A2</f>
         <v>1</v>
       </c>
       <c r="K2" s="7" t="s">
@@ -930,7 +930,7 @@
         <v>11.05</v>
       </c>
       <c r="F3" s="45">
-        <f>C3*E3</f>
+        <f t="shared" si="0"/>
         <v>110.5</v>
       </c>
       <c r="G3" s="22" t="s">
@@ -943,7 +943,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="41">
-        <f>A3</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K3" s="23" t="s">
@@ -967,7 +967,7 @@
         <v>2.35</v>
       </c>
       <c r="F4" s="45">
-        <f>C4*E4</f>
+        <f t="shared" si="0"/>
         <v>23.5</v>
       </c>
       <c r="G4" s="45" t="s">
@@ -980,7 +980,7 @@
         <v>11</v>
       </c>
       <c r="J4" s="41">
-        <f>A4</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K4" s="47" t="s">
@@ -1004,7 +1004,7 @@
         <v>10.050000000000001</v>
       </c>
       <c r="F5" s="45">
-        <f>C5*E5</f>
+        <f t="shared" si="0"/>
         <v>201</v>
       </c>
       <c r="G5" s="8" t="s">
@@ -1017,7 +1017,7 @@
         <v>11</v>
       </c>
       <c r="J5" s="57">
-        <f>A5</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K5" s="47" t="s">
@@ -1041,7 +1041,7 @@
         <v>3.85</v>
       </c>
       <c r="F6" s="45">
-        <f>C6*E6</f>
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="G6" s="45" t="s">
@@ -1054,7 +1054,7 @@
         <v>11</v>
       </c>
       <c r="J6" s="57">
-        <f>A6</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K6" s="9" t="s">
@@ -1078,7 +1078,7 @@
         <v>5.25</v>
       </c>
       <c r="F7" s="45">
-        <f>C7*E7</f>
+        <f t="shared" si="0"/>
         <v>52.5</v>
       </c>
       <c r="G7" s="45" t="s">
@@ -1091,7 +1091,7 @@
         <v>11</v>
       </c>
       <c r="J7" s="57">
-        <f>A7</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="K7" s="10" t="s">
@@ -1115,7 +1115,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="F8" s="45">
-        <f>C8*E8</f>
+        <f t="shared" si="0"/>
         <v>25.5</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1128,7 +1128,7 @@
         <v>11</v>
       </c>
       <c r="J8" s="57">
-        <f>A8</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="K8" s="49" t="s">
@@ -1152,7 +1152,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="F9" s="45">
-        <f>C9*E9</f>
+        <f t="shared" si="0"/>
         <v>17.399999999999999</v>
       </c>
       <c r="G9" s="45" t="s">
@@ -1165,7 +1165,7 @@
         <v>47</v>
       </c>
       <c r="J9" s="41">
-        <f>A9</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="K9" s="12" t="s">
@@ -1189,7 +1189,7 @@
         <v>0.40239999999999998</v>
       </c>
       <c r="F10" s="45">
-        <f>C10*E10</f>
+        <f t="shared" si="0"/>
         <v>4.024</v>
       </c>
       <c r="G10" s="45" t="s">
@@ -1202,7 +1202,7 @@
         <v>15</v>
       </c>
       <c r="J10" s="41">
-        <f>A10</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="K10" s="66" t="s">
@@ -1226,7 +1226,7 @@
         <v>0.12529999999999999</v>
       </c>
       <c r="F11" s="45">
-        <f>C11*E11</f>
+        <f t="shared" si="0"/>
         <v>12.53</v>
       </c>
       <c r="G11" s="40" t="s">
@@ -1239,7 +1239,7 @@
         <v>15</v>
       </c>
       <c r="J11" s="41">
-        <f>A11</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="K11" s="15" t="s">
@@ -1263,7 +1263,7 @@
         <v>0.2</v>
       </c>
       <c r="F12" s="45">
-        <f>C12*E12</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G12" s="59" t="s">
@@ -1276,7 +1276,7 @@
         <v>15</v>
       </c>
       <c r="J12" s="41">
-        <f>A12</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="K12" s="49" t="s">
@@ -1300,7 +1300,7 @@
         <v>3.8240000000000003E-2</v>
       </c>
       <c r="F13" s="45">
-        <f>C13*E13</f>
+        <f t="shared" si="0"/>
         <v>3.8240000000000003</v>
       </c>
       <c r="G13" s="45" t="s">
@@ -1313,7 +1313,7 @@
         <v>15</v>
       </c>
       <c r="J13" s="41">
-        <f>A13</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="K13" s="19" t="s">
@@ -1337,7 +1337,7 @@
         <v>0.37469999999999998</v>
       </c>
       <c r="F14" s="45">
-        <f>C14*E14</f>
+        <f t="shared" si="0"/>
         <v>18.734999999999999</v>
       </c>
       <c r="G14" s="45" t="s">
@@ -1350,7 +1350,7 @@
         <v>15</v>
       </c>
       <c r="J14" s="41">
-        <f>A14</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="K14" s="31" t="s">
@@ -1375,7 +1375,7 @@
         <v>2.47E-2</v>
       </c>
       <c r="F15" s="45">
-        <f>C15*E15</f>
+        <f t="shared" si="0"/>
         <v>2.4699999999999998</v>
       </c>
       <c r="G15" s="40" t="s">
@@ -1388,7 +1388,7 @@
         <v>15</v>
       </c>
       <c r="J15" s="41">
-        <f>A15</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="K15" s="47" t="s">
@@ -1412,7 +1412,7 @@
         <v>0.54759999999999998</v>
       </c>
       <c r="F16" s="45">
-        <f>C16*E16</f>
+        <f t="shared" si="0"/>
         <v>5.476</v>
       </c>
       <c r="G16" s="45" t="s">
@@ -1425,7 +1425,7 @@
         <v>15</v>
       </c>
       <c r="J16" s="41">
-        <f>A16</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="K16" s="28" t="s">
@@ -1449,7 +1449,7 @@
         <v>2.56</v>
       </c>
       <c r="F17" s="45">
-        <f>C17*E17</f>
+        <f t="shared" si="0"/>
         <v>25.6</v>
       </c>
       <c r="G17" s="39" t="s">
@@ -1462,7 +1462,7 @@
         <v>15</v>
       </c>
       <c r="J17" s="41">
-        <f>A17</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="K17" s="33" t="s">
@@ -1486,7 +1486,7 @@
         <v>0.6</v>
       </c>
       <c r="F18" s="45">
-        <f>C18*E18</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="G18" s="45" t="s">
@@ -1499,7 +1499,7 @@
         <v>15</v>
       </c>
       <c r="J18" s="41">
-        <f>A18</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="K18" s="47" t="s">
@@ -1523,7 +1523,7 @@
         <v>0.2016</v>
       </c>
       <c r="F19" s="45">
-        <f>C19*E19</f>
+        <f t="shared" si="0"/>
         <v>2.016</v>
       </c>
       <c r="G19" s="39" t="s">
@@ -1536,7 +1536,7 @@
         <v>15</v>
       </c>
       <c r="J19" s="41">
-        <f>A19</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="K19" s="35" t="s">
@@ -1560,7 +1560,7 @@
         <v>0.72</v>
       </c>
       <c r="F20" s="45">
-        <f>C20*E20</f>
+        <f t="shared" si="0"/>
         <v>7.1999999999999993</v>
       </c>
       <c r="G20" s="39" t="s">
@@ -1573,7 +1573,7 @@
         <v>15</v>
       </c>
       <c r="J20" s="41">
-        <f>A20</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="K20" s="47" t="s">
@@ -1597,7 +1597,7 @@
         <v>0.94399999999999995</v>
       </c>
       <c r="F21" s="45">
-        <f>C21*E21</f>
+        <f t="shared" si="0"/>
         <v>9.44</v>
       </c>
       <c r="G21" s="45" t="s">
@@ -1610,7 +1610,7 @@
         <v>15</v>
       </c>
       <c r="J21" s="41">
-        <f>A21</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="K21" s="47" t="s">
@@ -1634,7 +1634,7 @@
         <v>0.99199999999999999</v>
       </c>
       <c r="F22" s="45">
-        <f>C22*E22</f>
+        <f t="shared" si="0"/>
         <v>9.92</v>
       </c>
       <c r="G22" s="39" t="s">
@@ -1647,7 +1647,7 @@
         <v>15</v>
       </c>
       <c r="J22" s="41">
-        <f>A22</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="K22" s="47" t="s">
@@ -1671,7 +1671,7 @@
         <v>0.192</v>
       </c>
       <c r="F23" s="45">
-        <f>C23*E23</f>
+        <f t="shared" si="0"/>
         <v>1.92</v>
       </c>
       <c r="G23" s="39" t="s">
@@ -1684,7 +1684,7 @@
         <v>15</v>
       </c>
       <c r="J23" s="41">
-        <f>A23</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="K23" s="58" t="s">
@@ -1708,7 +1708,7 @@
         <v>0.498</v>
       </c>
       <c r="F24" s="45">
-        <f>C24*E24</f>
+        <f t="shared" si="0"/>
         <v>4.9800000000000004</v>
       </c>
       <c r="G24" s="45" t="s">
@@ -1721,7 +1721,7 @@
         <v>15</v>
       </c>
       <c r="J24" s="41">
-        <f>A24</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="K24" s="58" t="s">
@@ -1745,7 +1745,7 @@
         <v>48.28</v>
       </c>
       <c r="F25" s="45">
-        <f>C25*E25</f>
+        <f t="shared" si="0"/>
         <v>48.28</v>
       </c>
       <c r="G25" s="45" t="s">
@@ -1756,7 +1756,7 @@
         <v>74</v>
       </c>
       <c r="J25" s="57">
-        <f>A25</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="K25" s="58" t="s">
@@ -1779,7 +1779,7 @@
     <hyperlink ref="K8" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>